<commit_message>
Korrektur Testcode und Anpassung UML Diagramm
</commit_message>
<xml_diff>
--- a/src/org/hbrs/s1/ws22/uebung1/TemplateTestCase v1.6.xlsx
+++ b/src/org/hbrs/s1/ws22/uebung1/TemplateTestCase v1.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\IdeaProjects\codesSE2022\src\org\hbrs\s1\ws22\uebung1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C5D2E2-7B20-4A5B-9288-41C3DE51E7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297E21AF-E25A-4D57-8E07-0D190C62C636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Test Suite" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
   <si>
     <t>Testprozedur:</t>
   </si>
@@ -351,34 +351,28 @@
     <t>pos</t>
   </si>
   <si>
-    <t>ÄK_pos_1; 0 &lt; x &lt; 11 (nur  int)</t>
-  </si>
-  <si>
-    <t>-3.5</t>
-  </si>
-  <si>
     <t>neg</t>
   </si>
   <si>
     <t>"vier"</t>
   </si>
   <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>"Übersetzung der Zahl 3.5 nicht möglich. Version:... "</t>
-  </si>
-  <si>
-    <t>"Übersetzung der Zahl -2 nicht möglich. Version:... "</t>
-  </si>
-  <si>
-    <t>"f"</t>
-  </si>
-  <si>
-    <t>"Übersetzung der Zahl f nicht möglich. Version:... "</t>
-  </si>
-  <si>
-    <t>ÄK_neg_1; x&lt;0 || x&gt;10 ||  !int</t>
+    <t>"Übersetzung der Zahl 0 nicht möglich. Version: 1.0"</t>
+  </si>
+  <si>
+    <t>ÄK_pos_1; 0 &lt; x &lt; 11</t>
+  </si>
+  <si>
+    <t>ÄK_neg_1; x &lt; 0</t>
+  </si>
+  <si>
+    <t>ÄK_neg_2; x &gt; 10</t>
+  </si>
+  <si>
+    <t>"Übersetzung der Zahl -3 nicht möglich. Version: 1.0"</t>
+  </si>
+  <si>
+    <t>"Übersetzung der Zahl 15 nicht möglich. Version: 1.0"</t>
   </si>
 </sst>
 </file>
@@ -884,6 +878,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -893,9 +890,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1179,7 +1173,7 @@
   <dimension ref="C2:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -1204,9 +1198,9 @@
       <c r="C4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="56"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="27"/>
@@ -1215,12 +1209,12 @@
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="52" t="s">
+      <c r="C6" s="51"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="53"/>
+      <c r="F6" s="54"/>
     </row>
     <row r="7" spans="3:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="32" t="s">
@@ -1247,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.3">
@@ -1255,13 +1249,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="E9" s="50">
+        <v>-3</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.3">
@@ -1269,13 +1263,13 @@
         <v>3</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" s="24">
-        <v>-2</v>
+        <v>15</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.3">
@@ -1283,13 +1277,13 @@
         <v>4</v>
       </c>
       <c r="D11" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0</v>
+      </c>
+      <c r="F11" s="34" t="s">
         <v>65</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.3">
@@ -1340,7 +1334,7 @@
         <v>61</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E18" s="24">
         <v>4</v>
@@ -1354,20 +1348,26 @@
         <v>61</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="57" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="E19" s="50">
+        <v>-3</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="7"/>
+      <c r="D20" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="24">
+        <v>15</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="36" t="s">

</xml_diff>